<commit_message>
Updates on import prices, LCOEs, CFs, some data in generators DB and EET
- include a variable to change import prices and check their impact on oois
- correct some dates, name plate capacities and status for some generators
- Change the LCOEs and CF of almost all generators to reflect more real conditions. For instance, water was set at a very high price and it assumed a CF of 90%. In VIC this is not a realistic assumption.
- EET modified to include the changes on the extra paid when electricity has to be imported from other states. Also, price and capacity changes in solar were added.
</commit_message>
<xml_diff>
--- a/simulationData/1948_2019_Inflation_historic_Australia.xlsx
+++ b/simulationData/1948_2019_Inflation_historic_Australia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\gr4sp\experiments\simulationData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571ECA76-0EF5-429D-8050-D747EB2E4917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B51B78C-44F1-4B3E-89DD-1FE5CB86B1D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75F78C39-964A-4158-B6BA-BD969DC96C9F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Year</t>
   </si>
@@ -50,13 +50,22 @@
     <t>dec</t>
   </si>
   <si>
-    <t>ann</t>
-  </si>
-  <si>
     <t>INF%</t>
   </si>
   <si>
     <t>median</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>ann  (ave quarters)</t>
   </si>
 </sst>
 </file>
@@ -414,13 +423,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D1DD62-7CC2-4E44-8BA2-9E64252AED73}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="Q60" sqref="Q60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -439,7 +451,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -459,6 +471,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="F2" s="1">
+        <f>AVERAGE(B2:E2)</f>
         <v>1.6E-2</v>
       </c>
     </row>
@@ -479,7 +492,8 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="F3" s="1">
-        <v>1.9E-2</v>
+        <f t="shared" ref="F3:F66" si="0">AVERAGE(B3:E3)</f>
+        <v>1.925E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -499,7 +513,8 @@
         <v>1.9E-2</v>
       </c>
       <c r="F4" s="1">
-        <v>1.9E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.925E-2</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -520,7 +535,8 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F5" s="1">
-        <v>1.2999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.2749999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -540,6 +556,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="F6" s="1">
+        <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -560,7 +577,8 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="F7" s="1">
-        <v>2.5000000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.4749999999999998E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -580,7 +598,8 @@
         <v>2.7E-2</v>
       </c>
       <c r="F8" s="1">
-        <v>2.5000000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.4500000000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -600,7 +619,8 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F9" s="1">
-        <v>1.7000000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.7500000000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -620,6 +640,7 @@
         <v>0.03</v>
       </c>
       <c r="F10" s="1">
+        <f t="shared" si="0"/>
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
@@ -640,7 +661,8 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="F11" s="1">
-        <v>2.9000000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.9249999999999998E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -660,7 +682,8 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="F12" s="1">
-        <v>1.7000000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.7750000000000002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -680,7 +703,8 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="F13" s="1">
-        <v>4.3999999999999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.3500000000000004E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -700,7 +724,8 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="F14" s="1">
-        <v>2.3E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.325E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -720,7 +745,8 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="F15" s="1">
-        <v>3.5000000000000003E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.5500000000000004E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -740,6 +766,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="F16" s="1">
+        <f t="shared" si="0"/>
         <v>2.7E-2</v>
       </c>
     </row>
@@ -760,7 +787,8 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="F17" s="1">
-        <v>2.3E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.325E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -780,7 +808,8 @@
         <v>2.4E-2</v>
       </c>
       <c r="F18" s="1">
-        <v>2.7E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.7249999999999996E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -800,7 +829,8 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="F19" s="1">
-        <v>3.1E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.9749999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -820,7 +850,8 @@
         <v>3.1E-2</v>
       </c>
       <c r="F20" s="1">
-        <v>4.2999999999999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.4249999999999998E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -840,7 +871,8 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="F21" s="1">
-        <v>4.4999999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.4499999999999998E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -860,7 +892,8 @@
         <v>1.9E-2</v>
       </c>
       <c r="F22" s="1">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.4749999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -880,7 +913,8 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F23" s="1">
-        <v>7.0000000000000001E-3</v>
+        <f t="shared" si="0"/>
+        <v>8.7500000000000008E-3</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -900,7 +934,8 @@
         <v>-3.0000000000000001E-3</v>
       </c>
       <c r="F24" s="1">
-        <v>3.0000000000000001E-3</v>
+        <f t="shared" si="0"/>
+        <v>2.5000000000000005E-3</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -920,7 +955,8 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F25" s="1">
-        <v>2.5999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.6250000000000002E-2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -940,7 +976,8 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="F26" s="1">
-        <v>4.7E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.5999999999999992E-2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -959,8 +996,9 @@
       <c r="E27" s="1">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="F27" s="2">
-        <v>0.02</v>
+      <c r="F27" s="1">
+        <f t="shared" si="0"/>
+        <v>1.975E-2</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -980,7 +1018,8 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="F28" s="1">
-        <v>1.7000000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.7499999999999998E-2</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -999,8 +1038,9 @@
       <c r="E29" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F29" s="2">
-        <v>0.01</v>
+      <c r="F29" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002E-2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1020,7 +1060,8 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F30" s="1">
-        <v>3.1E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.175E-2</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1040,7 +1081,8 @@
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="F31" s="1">
-        <v>7.4999999999999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.3499999999999996E-2</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1060,7 +1102,8 @@
         <v>7.8E-2</v>
       </c>
       <c r="F32" s="1">
-        <v>7.3999999999999996E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.5250000000000011E-2</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1080,7 +1123,8 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="F33" s="1">
-        <v>7.2999999999999995E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.2250000000000009E-2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1100,7 +1144,8 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="F34" s="1">
-        <v>8.4000000000000005E-2</v>
+        <f t="shared" si="0"/>
+        <v>8.5500000000000007E-2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1120,7 +1165,8 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="F35" s="1">
-        <v>9.1999999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>9.0249999999999997E-2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1140,7 +1186,8 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="F36" s="1">
-        <v>6.5000000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.7250000000000004E-2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1159,7 +1206,8 @@
       <c r="E37" s="1">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="1">
+        <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
     </row>
@@ -1180,7 +1228,8 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="F38" s="1">
-        <v>0.10299999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.10075000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1200,7 +1249,8 @@
         <v>0.113</v>
       </c>
       <c r="F39" s="1">
-        <v>0.111</v>
+        <f t="shared" si="0"/>
+        <v>0.11349999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1220,7 +1270,8 @@
         <v>0.11</v>
       </c>
       <c r="F40" s="1">
-        <v>9.5000000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>9.4500000000000001E-2</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1240,7 +1291,8 @@
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="F41" s="1">
-        <v>0.105</v>
+        <f t="shared" si="0"/>
+        <v>0.10125000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1260,7 +1312,8 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="F42" s="1">
-        <v>9.0999999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>9.1249999999999998E-2</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1280,7 +1333,8 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="F43" s="1">
-        <v>7.9000000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>8.0250000000000002E-2</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1300,7 +1354,8 @@
         <v>9.4E-2</v>
       </c>
       <c r="F44" s="1">
-        <v>0.122</v>
+        <f t="shared" si="0"/>
+        <v>0.124</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1320,7 +1375,8 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="F45" s="1">
-        <v>0.13100000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.13300000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1340,7 +1396,8 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="F46" s="1">
-        <v>0.151</v>
+        <f t="shared" si="0"/>
+        <v>0.1525</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1360,7 +1417,8 @@
         <v>0.16700000000000001</v>
       </c>
       <c r="F47" s="1">
-        <v>0.158</v>
+        <f t="shared" si="0"/>
+        <v>0.15375000000000003</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1380,7 +1438,8 @@
         <v>0.125</v>
       </c>
       <c r="F48" s="1">
-        <v>9.0999999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>9.0749999999999997E-2</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1400,7 +1459,8 @@
         <v>4.7E-2</v>
       </c>
       <c r="F49" s="1">
-        <v>5.8000000000000003E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.0499999999999998E-2</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1420,7 +1480,8 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F50" s="1">
-        <v>6.0999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.1249999999999999E-2</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1440,7 +1501,8 @@
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="F51" s="1">
-        <v>3.2000000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.4500000000000003E-2</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1460,6 +1522,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="F52" s="1">
+        <f t="shared" si="0"/>
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
@@ -1480,7 +1543,8 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F53" s="1">
-        <v>3.4000000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1500,7 +1564,8 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="F54" s="1">
-        <v>3.5000000000000003E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.4750000000000003E-2</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1520,7 +1585,8 @@
         <v>2.4E-2</v>
       </c>
       <c r="F55" s="1">
-        <v>2.4E-2</v>
+        <f>AVERAGE(B55:E55)</f>
+        <v>3.3249999999999995E-2</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1540,7 +1606,8 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="F56" s="1">
-        <v>3.6999999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.4250000000000003E-2</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1560,7 +1627,8 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="F57" s="1">
-        <v>2.5000000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.8749999999999998E-2</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1580,7 +1648,8 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="F58" s="1">
-        <v>1.2999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.4999999999999997E-3</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1599,8 +1668,9 @@
       <c r="E59" s="2">
         <v>0</v>
       </c>
-      <c r="F59" s="2">
-        <v>0</v>
+      <c r="F59" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.2499999999999999E-3</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1620,7 +1690,8 @@
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <v>1.2999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1640,7 +1711,8 @@
         <v>0.04</v>
       </c>
       <c r="F61" s="1">
-        <v>4.1000000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.7250000000000005E-2</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1660,7 +1732,8 @@
         <v>2.7E-2</v>
       </c>
       <c r="F62" s="1">
-        <v>2.8000000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.0750000000000001E-2</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -1679,8 +1752,9 @@
       <c r="E63" s="1">
         <v>1.4E-2</v>
       </c>
-      <c r="F63" s="2">
-        <v>0</v>
+      <c r="F63" s="1">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1700,7 +1774,8 @@
         <v>1.4E-2</v>
       </c>
       <c r="F64" s="1">
-        <v>2.9000000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.9249999999999998E-2</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1720,7 +1795,8 @@
         <v>0.06</v>
       </c>
       <c r="F65" s="1">
-        <v>6.0999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.6999999999999995E-2</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1740,7 +1816,8 @@
         <v>3.1E-2</v>
       </c>
       <c r="F66" s="1">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.525E-2</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1760,6 +1837,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="F67" s="1">
+        <f t="shared" ref="F67:F72" si="1">AVERAGE(B67:E67)</f>
         <v>1.6E-2</v>
       </c>
     </row>
@@ -1780,7 +1858,8 @@
         <v>1.6E-2</v>
       </c>
       <c r="F68" s="1">
-        <v>4.9000000000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.5249999999999999E-2</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1800,7 +1879,8 @@
         <v>0.105</v>
       </c>
       <c r="F69" s="1">
-        <v>0.17299999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.17500000000000002</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1820,7 +1900,8 @@
         <v>0.23899999999999999</v>
       </c>
       <c r="F70" s="1">
-        <v>0.182</v>
+        <f t="shared" si="1"/>
+        <v>0.19324999999999998</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -1839,8 +1920,9 @@
       <c r="E71" s="1">
         <v>0.122</v>
       </c>
-      <c r="F71" s="2">
-        <v>0.1</v>
+      <c r="F71" s="1">
+        <f t="shared" si="1"/>
+        <v>8.6749999999999994E-2</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -1848,10 +1930,10 @@
         <v>1949</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D72" s="1">
         <v>0.108</v>
@@ -1860,16 +1942,44 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F72" s="1">
-        <v>1.105</v>
+        <f t="shared" si="1"/>
+        <v>9.35E-2</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
+        <v>6</v>
+      </c>
+      <c r="F75" s="1">
+        <f>MEDIAN(F2:F72)</f>
+        <v>3.3249999999999995E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
         <v>7</v>
       </c>
-      <c r="F75" s="1">
-        <f>MEDIAN(F2:F71)</f>
-        <v>3.3000000000000002E-2</v>
+      <c r="F76" s="1">
+        <f>AVERAGE(F2:F72)</f>
+        <v>5.0588028169014074E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" s="1">
+        <f>MAX(F2:F72)</f>
+        <v>0.19324999999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" s="1">
+        <f>MIN(F2:F72)</f>
+        <v>-3.2499999999999999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>